<commit_message>
syntax sugers used in jp template for no code
</commit_message>
<xml_diff>
--- a/dialbb/no_code/templates/ja/scenario.xlsx
+++ b/dialbb/no_code/templates/ja/scenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-nc-sample\ja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb2\dialbb\no_code\templates\ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE87ACC-CBE4-404F-889A-AD642E4C72B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCA47D0-4820-4E73-9F27-BAEA892F9C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
@@ -106,14 +106,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>_ne(#NE_Person, "")</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>_set(&amp;user_name, #NE_Person)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>名前を言った</t>
     <rPh sb="0" eb="2">
       <t>ナマエ</t>
@@ -281,24 +273,30 @@
       <t>ハンダン</t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>#NE_Person!= ""</t>
+  </si>
+  <si>
+    <t>user_name=#NE_Person</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -740,23 +738,23 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.625" style="5"/>
-    <col min="2" max="2" width="25.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.25" style="5" customWidth="1"/>
-    <col min="6" max="6" width="33.5" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.59765625" style="5"/>
+    <col min="2" max="2" width="25.46484375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.59765625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.86328125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.265625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="33.46484375" style="6" customWidth="1"/>
     <col min="7" max="7" width="39" style="6" customWidth="1"/>
-    <col min="8" max="8" width="37.875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.625" style="5"/>
+    <col min="8" max="8" width="37.86328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.59765625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -782,27 +780,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="7" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" s="7" customFormat="1" ht="42.75">
       <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="1:8" s="7" customFormat="1">
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
@@ -811,29 +809,29 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="9" customFormat="1" ht="57">
       <c r="B4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>17</v>
       </c>
       <c r="D4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="11" customFormat="1" ht="75" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="11" customFormat="1" ht="57">
       <c r="B5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>6</v>
@@ -841,74 +839,74 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="13" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="13" customFormat="1" ht="42.75">
       <c r="B6" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" s="14"/>
       <c r="F6" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="13" customFormat="1" ht="37.5" x14ac:dyDescent="0.4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="13" customFormat="1" ht="28.5">
       <c r="B7" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="F7" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="13" customFormat="1">
       <c r="B8" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" ht="93.75" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="3" customFormat="1" ht="99.75">
       <c r="B9" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:8" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" s="3" customFormat="1" ht="71.25">
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" ht="56.25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" s="1" customFormat="1" ht="42.75">
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
jp no-code template app updated
</commit_message>
<xml_diff>
--- a/dialbb/no_code/templates/ja/scenario.xlsx
+++ b/dialbb/no_code/templates/ja/scenario.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,20 +484,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>こんにちは。私はチャットボットです。よろしければお名前を教えて頂けますか？</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>田中です。</t>
-        </is>
-      </c>
+          <t xml:space="preserve">こんにちは。私はチャットボットです。気軽にお話しましょう。料理は良くする方ですか？ </t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>$ユーザが名前を言ったか判断してください$</t>
-        </is>
-      </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
@@ -509,13 +501,22 @@
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>#initial</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
+          <t>state1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">$あなたの次の発話を30文字以内で生成してください。$
+</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>$ユーザが飽きているかどうか判断してください$</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
@@ -530,18 +531,18 @@
           <t>state1</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>ありがとうございます。$ユーザの名前を呼ぶ発話を生成してください$、今日はラーメンについて教えて下さい。ラーメンはよく食べますか？</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>TS&gt;5</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>state3</t>
+          <t>state2</t>
         </is>
       </c>
     </row>
@@ -549,147 +550,73 @@
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr">
         <is>
-          <t>state2</t>
+          <t>#error</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>すみません、ちょっと理解できませんでした。今日はラーメンについて教えて下さい。ラーメンはよく食べますか？</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>はい、よく食べます。</t>
-        </is>
-      </c>
+          <t>申し訳ありません。内部エラーがおきてしまいました。今日はありがとうございました。</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>state3</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr">
         <is>
-          <t>state3</t>
+          <t>#final_state1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>$ラーメンに関する雑談を続けるために次の発話を30文字以内で生成してください。$</t>
+          <t>$それまでの発話に続けて、対話を終わらせる発話を30文字以内で生成してください。$</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>TT&gt;10</t>
-        </is>
-      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>#final_state1</t>
-        </is>
-      </c>
+      <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
       <c r="B7" t="inlineStr">
         <is>
-          <t>state3</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
+          <t>state2</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">$$$
+# 状況
+{situation}
+# あなたのペルソナ
+{persona}
+# 今までの対話
+{dialogue_history}
+# タスク
+料理以外の話に関して雑談をするために、あなたの次の発話を30文字以内で生成してください。
+$$$ 
+</t>
+        </is>
+      </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$ユーザが会話に飽きているかどうかを判断してください。$</t>
+          <t>TT&gt;10</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>#final_state2</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>state3</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>state3</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr">
-        <is>
           <t>#final_state1</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>$それまでの会話につづけた発話をするとともに、時間になったので会話を終わることを伝える発話を50文字で生成してください。$本日はありがとうございました。</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>#final_state2</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>$それまでの対話に続けて、つまらない話を続けたことを詫び、会話を終わらせてください。$本日はありがとうございました。</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>#error</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>申し訳ありません。内部エラーがおきてしまいました。今日はありがとうございました。</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>